<commit_message>
excel test is updated
</commit_message>
<xml_diff>
--- a/excel_test.xlsx
+++ b/excel_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeliH\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeliH\Documents\GitHub\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +389,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -401,6 +401,57 @@
       </c>
       <c r="D1" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>4234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>423</v>
+      </c>
+      <c r="G8" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>32423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>